<commit_message>
BOM and fixed pcb
</commit_message>
<xml_diff>
--- a/encoder.xlsx
+++ b/encoder.xlsx
@@ -1,59 +1,150 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26216"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\file\Usersg$\gal65\Home\My Documents\~Masters\Encoder PCB\encoder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucliveac-my.sharepoint.com/personal/gal65_uclive_ac_nz/Documents/Masters 2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{8BE1659B-6AAE-4DC5-97C6-DB7F54069E69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{52E42B52-EDAB-4145-896C-542D08122BE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="encoder" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Id;"Designator";"Package";"Quantity";"Designation";"Supplier and ref";</t>
-  </si>
-  <si>
-    <t>1;"J1";"BM04B-SURS-TFLFSN";1;"BM04B-SURS-TFLFSN";;;</t>
-  </si>
-  <si>
-    <t>2;"C2";"C_0603_1608Metric";1;"10uF";;;</t>
-  </si>
-  <si>
-    <t>3;"U1";"SOIC127P600X175-8N";1;"AS5600-ASOT";;;</t>
-  </si>
-  <si>
-    <t>4;"H1</t>
-  </si>
-  <si>
-    <t>H2";"MountingHole_2.7mm_M2.5_ISO7380";2;"MountingHole";;;</t>
-  </si>
-  <si>
-    <t>5;"R1</t>
-  </si>
-  <si>
-    <t>R2";"R_0603_1608Metric_Pad0.98x0.95mm_HandSolder";2;"R";;;</t>
-  </si>
-  <si>
-    <t>6;"C1";"C_0603_1608Metric";1;"100nF";;;</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
+  <si>
+    <t>Component Count:</t>
+  </si>
+  <si>
+    <t>Ref</t>
+  </si>
+  <si>
+    <t>Qnty</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Cmp name</t>
+  </si>
+  <si>
+    <t>Footprint</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>Vendor part number</t>
+  </si>
+  <si>
+    <t>Received</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1, </t>
+  </si>
+  <si>
+    <t>100nF</t>
+  </si>
+  <si>
+    <t>C_Small</t>
+  </si>
+  <si>
+    <t>Capacitor_SMD:C_0603_1608Metric</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>SMT Lab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C2, </t>
+  </si>
+  <si>
+    <t>10uF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H1, H2, </t>
+  </si>
+  <si>
+    <t>MountingHole</t>
+  </si>
+  <si>
+    <t>MountingHole:MountingHole_2.7mm_M2.5_ISO7380</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J1, </t>
+  </si>
+  <si>
+    <t>BM04B-SURS-TFLFSN</t>
+  </si>
+  <si>
+    <t>BM04B:BM04B-SURS-TFLFSN</t>
+  </si>
+  <si>
+    <t>LCSC</t>
+  </si>
+  <si>
+    <t>C495551</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R1, R2, </t>
+  </si>
+  <si>
+    <t>0R</t>
+  </si>
+  <si>
+    <t>Resistor_SMD:R_0603_1608Metric_Pad0.98x0.95mm_HandSolder</t>
+  </si>
+  <si>
+    <t>C17168</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U1, </t>
+  </si>
+  <si>
+    <t>AS5600-ASOT</t>
+  </si>
+  <si>
+    <t>AS5600:SOIC127P600X175-8N</t>
+  </si>
+  <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>AS5600-ASOTCT-ND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -886,58 +977,204 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="65.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="59.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
         <v>2</v>
       </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>